<commit_message>
#1 database architecture changes
</commit_message>
<xml_diff>
--- a/doc/prj.xlsx
+++ b/doc/prj.xlsx
@@ -9,21 +9,17 @@
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
     <sheet name="Test" sheetId="2" r:id="rId2"/>
-    <sheet name="Links" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="146">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>выданный номер</t>
-  </si>
-  <si>
     <t>login</t>
   </si>
   <si>
@@ -40,9 +36,6 @@
   </si>
   <si>
     <t>NN</t>
-  </si>
-  <si>
-    <t>UQ, NN</t>
   </si>
   <si>
     <t>тип</t>
@@ -152,9 +145,6 @@
     <t>rate</t>
   </si>
   <si>
-    <t>fullName</t>
-  </si>
-  <si>
     <t>phoneNum</t>
   </si>
   <si>
@@ -297,18 +287,6 @@
   </si>
   <si>
     <t>subscriber</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>ул. Полярная, д. 1</t>
-  </si>
-  <si>
-    <t>ул. Полярная, д. 2</t>
-  </si>
-  <si>
-    <t>https://dev.mysql.com/doc/refman/5.6/en/enum.html</t>
   </si>
   <si>
     <t>administratorID</t>
@@ -526,9 +504,6 @@
     </r>
   </si>
   <si>
-    <t>U - Dao обновление не всех полей (типа id и тп)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">subscribers </t>
     </r>
@@ -571,7 +546,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">administrators </t>
+      <t xml:space="preserve">provided_services  </t>
     </r>
     <r>
       <rPr>
@@ -607,7 +582,163 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/*список администраторов</t>
+      <t>/* предоставляемые услуги */</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">calls </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRU</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* звонки */</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">calling_rates </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* тарифы на звонки */</t>
+    </r>
+  </si>
+  <si>
+    <t>isActive</t>
+  </si>
+  <si>
+    <t>surname</t>
+  </si>
+  <si>
+    <t>patronymic</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>prefixID</t>
+  </si>
+  <si>
+    <t>passportID</t>
+  </si>
+  <si>
+    <t>personalID</t>
+  </si>
+  <si>
+    <t>личный номер сотрудника</t>
+  </si>
+  <si>
+    <t>true|false активен|заблокирован</t>
+  </si>
+  <si>
+    <t>префикс тел. номера</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">prefixes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* префиксы телефонных номеров</t>
     </r>
     <r>
       <rPr>
@@ -625,30 +756,6 @@
       <rPr>
         <i/>
         <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>админы создаются вручную?</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
         <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -659,8 +766,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">provided_services  </t>
+    <t>город</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">administrators </t>
     </r>
     <r>
       <rPr>
@@ -696,103 +806,42 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/* предоставляемые услуги */</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">calls </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRU</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/* звонки */</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">calling_rates </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRUD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/* тарифы на звонки */</t>
-    </r>
-  </si>
-  <si>
-    <t>true|false</t>
-  </si>
-  <si>
-    <t>isActive</t>
+      <t>/*список администраторов */</t>
+    </r>
+  </si>
+  <si>
+    <t>идентификационный номер паспорта</t>
+  </si>
+  <si>
+    <t>NN, UQ(сост)</t>
+  </si>
+  <si>
+    <t>префикс тел. номера, составной уникальный ключ</t>
+  </si>
+  <si>
+    <t>телефонный номер, составной уникальный ключ</t>
+  </si>
+  <si>
+    <t>0101ASJL2</t>
+  </si>
+  <si>
+    <t>0101ASJL3</t>
+  </si>
+  <si>
+    <t>surname+name+patronymic</t>
+  </si>
+  <si>
+    <t>210045, ул. Полярная, д. 1</t>
+  </si>
+  <si>
+    <t>210007, ул. Заполярная, д. 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,15 +863,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -950,7 +990,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1043,12 +1083,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
@@ -1060,29 +1122,38 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1111,6 +1182,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1424,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L46"/>
+  <dimension ref="B2:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,713 +1521,821 @@
     <col min="7" max="7" width="7.140625" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.7109375" style="22" customWidth="1"/>
+    <col min="12" max="12" width="51.28515625" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="21" t="s">
+      <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30"/>
+      <c r="B4" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="23"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="27"/>
+      <c r="B8" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="27" t="s">
-        <v>115</v>
-      </c>
+      <c r="B9" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="28"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="44"/>
+      <c r="H16" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="41"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="23"/>
+      <c r="H17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="23"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="27"/>
+      <c r="L18" s="34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="23"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H20" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="30"/>
+      <c r="L20" s="31"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H21" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H22" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="K22" s="17"/>
+      <c r="L22" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="47"/>
+    </row>
+    <row r="27" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="23" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-      <c r="H13" s="32" t="s">
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="34"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="23"/>
-      <c r="H14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L14" s="23"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="23"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>126</v>
-      </c>
-      <c r="F17" s="26"/>
-      <c r="H17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="23"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F18" s="26"/>
-      <c r="H18" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K18" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="L18" s="24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
-      <c r="H22" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="30"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="23"/>
-      <c r="H23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="23"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C28" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="23"/>
-      <c r="H24" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K24" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="L24" s="25"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="23"/>
-      <c r="H25" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="L25" s="25"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="K26" s="1"/>
-      <c r="L26" s="23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="K27" s="1"/>
-      <c r="L27" s="23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="23" t="s">
+      <c r="E28" s="27"/>
+      <c r="F28" s="34" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="35" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L29" s="26"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F30" s="26"/>
-      <c r="L30" s="26"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30"/>
-      <c r="H32" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="30"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="37"/>
+      <c r="H32" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="37"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="23" t="s">
-        <v>116</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F33" s="23"/>
       <c r="H33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L33" s="23"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="23"/>
       <c r="H34" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J34" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="L34" s="25"/>
+        <v>13</v>
+      </c>
+      <c r="L34" s="24"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>108</v>
+        <v>19</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I35" s="1" t="s">
+      <c r="F35" s="23"/>
+      <c r="H35" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="24"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K37" s="1"/>
+      <c r="L37" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K35" s="1"/>
-      <c r="L35" s="23"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K36" s="1"/>
-      <c r="L36" s="23"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J37" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="K37" s="1"/>
-      <c r="L37" s="23"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H38" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="I38" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="J38" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K38" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="L38" s="25" t="s">
-        <v>116</v>
-      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L39" s="25"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F40" s="26"/>
+      <c r="F40" s="25"/>
+      <c r="L40" s="25"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="30"/>
-      <c r="H42" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
+      <c r="B42" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="37"/>
+      <c r="H42" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="37"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" s="23"/>
+        <v>12</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>109</v>
+      </c>
       <c r="H43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J43" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" s="23"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L43" s="23"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="19" t="s">
+      <c r="D44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="23"/>
+      <c r="H44" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="J44" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K44" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L44" s="24"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K45" s="1"/>
+      <c r="L45" s="23"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K46" s="1"/>
+      <c r="L46" s="23"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J47" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K47" s="1"/>
+      <c r="L47" s="23"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H48" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I48" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="J48" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K48" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L48" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F50" s="25"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="37"/>
+      <c r="H52" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="23"/>
+      <c r="H53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L53" s="23"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="24"/>
+      <c r="H54" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" s="25"/>
-      <c r="H44" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K44" s="1"/>
-      <c r="L44" s="23"/>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="23"/>
-      <c r="H45" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K45" s="1"/>
-      <c r="L45" s="23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C46" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="H46" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="I46" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="J46" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K46" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="L46" s="25"/>
+      <c r="J54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K54" s="1"/>
+      <c r="L54" s="23"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="23"/>
+      <c r="H55" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K55" s="1"/>
+      <c r="L55" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H56" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="I56" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="J56" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K56" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L56" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="H52:L52"/>
+    <mergeCell ref="B52:F52"/>
     <mergeCell ref="H42:L42"/>
     <mergeCell ref="B42:F42"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2158,8 +2346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,11 +2355,10 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.42578125" customWidth="1"/>
     <col min="10" max="10" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
@@ -2182,246 +2369,266 @@
     <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1">
         <v>123</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>49</v>
+      <c r="E4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1">
         <v>456</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>50</v>
+      <c r="E5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>17</v>
+        <v>129</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
+      <c r="C11" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="6">
+        <v>29566</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="6">
-        <v>29566</v>
-      </c>
-      <c r="G11" s="1">
+        <v>144</v>
+      </c>
+      <c r="F11" s="1">
+        <v>212</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>2</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>51</v>
+      <c r="C12" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="6">
+        <v>28105</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="6">
-        <v>28105</v>
-      </c>
-      <c r="G12" s="1">
+        <v>145</v>
+      </c>
+      <c r="F12" s="1">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="29"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="36"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>130</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
         <v>3</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>62</v>
+      <c r="C17" s="1">
+        <v>54821324</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <v>4</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>62</v>
+      <c r="C18" s="1">
+        <v>54821325</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
-      <c r="J20" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="30"/>
+      <c r="B20" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="37"/>
+      <c r="J20" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="37"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="N21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
@@ -2429,10 +2636,10 @@
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E22" s="1">
         <v>3</v>
@@ -2441,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J22" s="1">
         <v>1</v>
@@ -2456,7 +2663,7 @@
         <v>43040</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2464,10 +2671,10 @@
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E23" s="1">
         <v>0.5</v>
@@ -2476,7 +2683,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J23" s="1">
         <v>1</v>
@@ -2491,7 +2698,7 @@
         <v>43040</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -2499,10 +2706,10 @@
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E24" s="1">
         <v>3.05</v>
@@ -2511,7 +2718,7 @@
         <v>5.67</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J24" s="1">
         <v>2</v>
@@ -2526,7 +2733,7 @@
         <v>43042</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
@@ -2534,10 +2741,10 @@
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -2546,7 +2753,7 @@
         <v>100</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J25" s="1">
         <v>3</v>
@@ -2561,7 +2768,7 @@
         <v>43043</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
@@ -2569,10 +2776,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E26" s="1">
         <v>0.85</v>
@@ -2581,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J26" s="1">
         <v>4</v>
@@ -2596,7 +2803,7 @@
         <v>43040</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
@@ -2613,51 +2820,51 @@
         <v>43040</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30"/>
-      <c r="J30" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
+      <c r="B30" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="37"/>
+      <c r="J30" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
@@ -2668,13 +2875,13 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G32" s="15">
         <v>1</v>
@@ -2683,7 +2890,7 @@
         <v>1</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L32" s="1">
         <v>0</v>
@@ -2697,13 +2904,13 @@
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G33" s="15">
         <v>2</v>
@@ -2712,7 +2919,7 @@
         <v>2</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L33" s="1">
         <v>0.03</v>
@@ -2726,13 +2933,13 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G34" s="15">
         <v>3</v>
@@ -2741,7 +2948,7 @@
         <v>3</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L34" s="1">
         <v>0.15</v>
@@ -2755,13 +2962,13 @@
         <v>2</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G35" s="15">
         <v>1</v>
@@ -2775,56 +2982,56 @@
         <v>2</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G36" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="J40" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
+      <c r="B40" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="J40" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="K40" s="38"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J41" s="17" t="s">
         <v>0</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L41" s="17" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="M41" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
@@ -2835,7 +3042,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E42" s="1">
         <v>16.77</v>
@@ -2844,10 +3051,10 @@
         <v>1</v>
       </c>
       <c r="K42" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="M42" s="15">
         <v>1</v>
@@ -2861,7 +3068,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E43" s="1">
         <v>16.77</v>
@@ -2882,24 +3089,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
providedServicesDao + providedServicesService impl
</commit_message>
<xml_diff>
--- a/doc/prj.xlsx
+++ b/doc/prj.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\Java\Station\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="19320" windowHeight="7995"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="147">
   <si>
     <t>id</t>
   </si>
@@ -836,11 +841,14 @@
   <si>
     <t>210007, ул. Заполярная, д. 2</t>
   </si>
+  <si>
+    <t>+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1220,7 +1228,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1253,9 +1261,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1288,6 +1313,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1464,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L56"/>
+  <dimension ref="B2:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,7 +1528,7 @@
     <col min="12" max="12" width="51.28515625" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1518,7 +1560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
         <v>115</v>
       </c>
@@ -1526,8 +1568,11 @@
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
       <c r="F4" s="30"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1544,7 +1589,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1557,7 +1602,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="23"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1572,7 +1617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>124</v>
       </c>
@@ -1585,7 +1630,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="26"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1598,7 +1643,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="26"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>125</v>
       </c>
@@ -1611,7 +1656,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="26"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
@@ -1626,7 +1671,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>123</v>
       </c>
@@ -1641,7 +1686,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="35" t="s">
         <v>136</v>
       </c>
@@ -1649,6 +1694,9 @@
       <c r="D16" s="36"/>
       <c r="E16" s="36"/>
       <c r="F16" s="37"/>
+      <c r="G16" t="s">
+        <v>146</v>
+      </c>
       <c r="H16" s="32" t="s">
         <v>119</v>
       </c>
@@ -1656,6 +1704,9 @@
       <c r="J16" s="33"/>
       <c r="K16" s="33"/>
       <c r="L16" s="34"/>
+      <c r="M16" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">

</xml_diff>

<commit_message>
servicesDao + servicesService impl
</commit_message>
<xml_diff>
--- a/doc/prj.xlsx
+++ b/doc/prj.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="147">
   <si>
     <t>id</t>
   </si>
@@ -1509,7 +1509,7 @@
   <dimension ref="B2:M56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,7 +1708,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>0</v>
       </c>
@@ -1736,7 +1736,7 @@
       </c>
       <c r="L17" s="24"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>130</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1790,7 +1790,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="27"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H20" s="1" t="s">
         <v>15</v>
       </c>
@@ -1803,7 +1803,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="27"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H21" s="19" t="s">
         <v>128</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H22" s="1" t="s">
         <v>38</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H23" s="19" t="s">
         <v>86</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="35" t="s">
         <v>134</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="E26" s="36"/>
       <c r="F26" s="37"/>
     </row>
-    <row r="27" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>126</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>127</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="28" t="s">
         <v>120</v>
       </c>
@@ -1901,6 +1901,9 @@
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
       <c r="F32" s="30"/>
+      <c r="G32" t="s">
+        <v>146</v>
+      </c>
       <c r="H32" s="28" t="s">
         <v>117</v>
       </c>
@@ -1908,6 +1911,9 @@
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
       <c r="L32" s="30"/>
+      <c r="M32" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">

</xml_diff>

<commit_message>
CallRateDao + CallRateService impl CallDao + CallService impl
</commit_message>
<xml_diff>
--- a/doc/prj.xlsx
+++ b/doc/prj.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="147">
   <si>
     <t>id</t>
   </si>
@@ -1508,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,6 +2081,9 @@
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
       <c r="F42" s="30"/>
+      <c r="G42" t="s">
+        <v>146</v>
+      </c>
       <c r="H42" s="28" t="s">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
InvoiceDao + InvoiceService impl
</commit_message>
<xml_diff>
--- a/doc/prj.xlsx
+++ b/doc/prj.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="147">
   <si>
     <t>id</t>
   </si>
@@ -481,7 +481,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">invoices </t>
+      <t xml:space="preserve">subscribers </t>
     </r>
     <r>
       <rPr>
@@ -493,7 +493,343 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">CR </t>
+      <t>CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* абоненты */</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">provided_services  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* предоставляемые услуги */</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">calls </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRU</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* звонки */</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">calling_rates </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* тарифы на звонки */</t>
+    </r>
+  </si>
+  <si>
+    <t>isActive</t>
+  </si>
+  <si>
+    <t>surname</t>
+  </si>
+  <si>
+    <t>patronymic</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>prefixID</t>
+  </si>
+  <si>
+    <t>passportID</t>
+  </si>
+  <si>
+    <t>personalID</t>
+  </si>
+  <si>
+    <t>личный номер сотрудника</t>
+  </si>
+  <si>
+    <t>true|false активен|заблокирован</t>
+  </si>
+  <si>
+    <t>префикс тел. номера</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">prefixes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* префиксы телефонных номеров</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*/</t>
+    </r>
+  </si>
+  <si>
+    <t>город</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">administrators </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/*список администраторов */</t>
+    </r>
+  </si>
+  <si>
+    <t>идентификационный номер паспорта</t>
+  </si>
+  <si>
+    <t>NN, UQ(сост)</t>
+  </si>
+  <si>
+    <t>префикс тел. номера, составной уникальный ключ</t>
+  </si>
+  <si>
+    <t>телефонный номер, составной уникальный ключ</t>
+  </si>
+  <si>
+    <t>0101ASJL2</t>
+  </si>
+  <si>
+    <t>0101ASJL3</t>
+  </si>
+  <si>
+    <t>surname+name+patronymic</t>
+  </si>
+  <si>
+    <t>210045, ул. Полярная, д. 1</t>
+  </si>
+  <si>
+    <t>210007, ул. Заполярная, д. 2</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">invoices </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CRUD </t>
     </r>
     <r>
       <rPr>
@@ -507,342 +843,6 @@
       </rPr>
       <t>/* счета */</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">subscribers </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRUD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/* абоненты */</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">provided_services  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRUD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/* предоставляемые услуги */</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">calls </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRU</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/* звонки */</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">calling_rates </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRUD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/* тарифы на звонки */</t>
-    </r>
-  </si>
-  <si>
-    <t>isActive</t>
-  </si>
-  <si>
-    <t>surname</t>
-  </si>
-  <si>
-    <t>patronymic</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>prefixID</t>
-  </si>
-  <si>
-    <t>passportID</t>
-  </si>
-  <si>
-    <t>personalID</t>
-  </si>
-  <si>
-    <t>личный номер сотрудника</t>
-  </si>
-  <si>
-    <t>true|false активен|заблокирован</t>
-  </si>
-  <si>
-    <t>префикс тел. номера</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">prefixes </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRUD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/* префиксы телефонных номеров</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*/</t>
-    </r>
-  </si>
-  <si>
-    <t>город</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">administrators </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRUD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/*список администраторов */</t>
-    </r>
-  </si>
-  <si>
-    <t>идентификационный номер паспорта</t>
-  </si>
-  <si>
-    <t>NN, UQ(сост)</t>
-  </si>
-  <si>
-    <t>префикс тел. номера, составной уникальный ключ</t>
-  </si>
-  <si>
-    <t>телефонный номер, составной уникальный ключ</t>
-  </si>
-  <si>
-    <t>0101ASJL2</t>
-  </si>
-  <si>
-    <t>0101ASJL3</t>
-  </si>
-  <si>
-    <t>surname+name+patronymic</t>
-  </si>
-  <si>
-    <t>210045, ул. Полярная, д. 1</t>
-  </si>
-  <si>
-    <t>210007, ул. Заполярная, д. 2</t>
-  </si>
-  <si>
-    <t>+</t>
   </si>
 </sst>
 </file>
@@ -1508,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,7 +1569,7 @@
       <c r="E4" s="29"/>
       <c r="F4" s="30"/>
       <c r="G4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>103</v>
@@ -1645,7 +1645,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>103</v>
@@ -1673,7 +1673,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>112</v>
@@ -1683,29 +1683,29 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C16" s="36"/>
       <c r="D16" s="36"/>
       <c r="E16" s="36"/>
       <c r="F16" s="37"/>
       <c r="G16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I16" s="33"/>
       <c r="J16" s="33"/>
       <c r="K16" s="33"/>
       <c r="L16" s="34"/>
       <c r="M16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
@@ -1738,7 +1738,7 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>92</v>
@@ -1748,10 +1748,10 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>102</v>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -1805,19 +1805,19 @@
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H21" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>92</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K21" s="19" t="s">
         <v>13</v>
       </c>
       <c r="L21" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
@@ -1828,11 +1828,11 @@
         <v>92</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
@@ -1854,7 +1854,7 @@
     </row>
     <row r="26" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C26" s="36"/>
       <c r="D26" s="36"/>
@@ -1863,7 +1863,7 @@
     </row>
     <row r="27" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>92</v>
@@ -1875,12 +1875,12 @@
         <v>12</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>102</v>
@@ -1890,19 +1890,19 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
       <c r="F32" s="30"/>
       <c r="G32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H32" s="28" t="s">
         <v>117</v>
@@ -1912,10 +1912,10 @@
       <c r="K32" s="29"/>
       <c r="L32" s="30"/>
       <c r="M32" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>0</v>
       </c>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="L33" s="23"/>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>17</v>
       </c>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="L34" s="24"/>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>19</v>
       </c>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="L35" s="24"/>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>96</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>95</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>62</v>
       </c>
@@ -2066,33 +2066,36 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L39" s="25"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F40" s="25"/>
       <c r="L40" s="25"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C42" s="29"/>
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
       <c r="F42" s="30"/>
       <c r="G42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H42" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I42" s="29"/>
       <c r="J42" s="29"/>
       <c r="K42" s="29"/>
       <c r="L42" s="30"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>0</v>
       </c>
@@ -2122,7 +2125,7 @@
       </c>
       <c r="L43" s="23"/>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>17</v>
       </c>
@@ -2148,7 +2151,7 @@
       </c>
       <c r="L44" s="24"/>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>37</v>
       </c>
@@ -2174,7 +2177,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="23"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H46" s="1" t="s">
         <v>34</v>
       </c>
@@ -2187,7 +2190,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="23"/>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H47" s="1" t="s">
         <v>35</v>
       </c>
@@ -2200,7 +2203,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="23"/>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H48" s="19" t="s">
         <v>36</v>
       </c>
@@ -2222,12 +2225,15 @@
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="28" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
       <c r="E52" s="29"/>
       <c r="F52" s="30"/>
+      <c r="G52" t="s">
+        <v>145</v>
+      </c>
       <c r="H52" s="31" t="s">
         <v>116</v>
       </c>
@@ -2410,13 +2416,13 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2495,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>10</v>
@@ -2504,7 +2510,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>38</v>
@@ -2518,13 +2524,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11" s="6">
         <v>29566</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F11" s="1">
         <v>212</v>
@@ -2541,13 +2547,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D12" s="6">
         <v>28105</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F12" s="1">
         <v>17</v>
@@ -2571,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
PaymentDao + PaymentService impl
</commit_message>
<xml_diff>
--- a/doc/prj.xlsx
+++ b/doc/prj.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="147">
   <si>
     <t>id</t>
   </si>
@@ -1508,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2220,10 +2220,10 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F50" s="25"/>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="28" t="s">
         <v>146</v>
       </c>
@@ -2241,8 +2241,11 @@
       <c r="J52" s="31"/>
       <c r="K52" s="31"/>
       <c r="L52" s="31"/>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>0</v>
       </c>
@@ -2270,7 +2273,7 @@
       </c>
       <c r="L53" s="23"/>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>21</v>
       </c>
@@ -2296,7 +2299,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="23"/>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
         <v>31</v>
       </c>
@@ -2322,7 +2325,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
PrefixDao + PrefixService impl
</commit_message>
<xml_diff>
--- a/doc/prj.xlsx
+++ b/doc/prj.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="146">
   <si>
     <t>id</t>
   </si>
@@ -811,9 +811,6 @@
   </si>
   <si>
     <t>210007, ул. Заполярная, д. 2</t>
-  </si>
-  <si>
-    <t>+</t>
   </si>
   <si>
     <r>
@@ -1506,10 +1503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M56"/>
+  <dimension ref="B2:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1528,7 +1525,7 @@
     <col min="12" max="12" width="51.28515625" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1560,7 +1557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
         <v>115</v>
       </c>
@@ -1568,11 +1565,8 @@
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
       <c r="F4" s="30"/>
-      <c r="G4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1589,7 +1583,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1602,7 +1596,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="23"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1617,7 +1611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>123</v>
       </c>
@@ -1630,7 +1624,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="26"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1643,7 +1637,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="26"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>124</v>
       </c>
@@ -1656,7 +1650,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="26"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
@@ -1671,7 +1665,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>122</v>
       </c>
@@ -1686,7 +1680,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="35" t="s">
         <v>135</v>
       </c>
@@ -1694,9 +1688,6 @@
       <c r="D16" s="36"/>
       <c r="E16" s="36"/>
       <c r="F16" s="37"/>
-      <c r="G16" t="s">
-        <v>145</v>
-      </c>
       <c r="H16" s="32" t="s">
         <v>118</v>
       </c>
@@ -1704,11 +1695,8 @@
       <c r="J16" s="33"/>
       <c r="K16" s="33"/>
       <c r="L16" s="34"/>
-      <c r="M16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>0</v>
       </c>
@@ -1736,7 +1724,7 @@
       </c>
       <c r="L17" s="24"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>129</v>
       </c>
@@ -1764,7 +1752,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1790,7 +1778,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="27"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H20" s="1" t="s">
         <v>15</v>
       </c>
@@ -1803,7 +1791,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="27"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H21" s="19" t="s">
         <v>127</v>
       </c>
@@ -1820,7 +1808,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H22" s="1" t="s">
         <v>38</v>
       </c>
@@ -1835,7 +1823,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H23" s="19" t="s">
         <v>86</v>
       </c>
@@ -1852,7 +1840,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="35" t="s">
         <v>133</v>
       </c>
@@ -1861,7 +1849,7 @@
       <c r="E26" s="36"/>
       <c r="F26" s="37"/>
     </row>
-    <row r="27" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>125</v>
       </c>
@@ -1878,7 +1866,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>126</v>
       </c>
@@ -1893,7 +1881,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="28" t="s">
         <v>119</v>
       </c>
@@ -1901,9 +1889,6 @@
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
       <c r="F32" s="30"/>
-      <c r="G32" t="s">
-        <v>145</v>
-      </c>
       <c r="H32" s="28" t="s">
         <v>117</v>
       </c>
@@ -1911,11 +1896,8 @@
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
       <c r="L32" s="30"/>
-      <c r="M32" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>0</v>
       </c>
@@ -1943,7 +1925,7 @@
       </c>
       <c r="L33" s="23"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>17</v>
       </c>
@@ -1969,7 +1951,7 @@
       </c>
       <c r="L34" s="24"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>19</v>
       </c>
@@ -1995,7 +1977,7 @@
       </c>
       <c r="L35" s="24"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>96</v>
       </c>
@@ -2023,7 +2005,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>95</v>
       </c>
@@ -2051,7 +2033,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>62</v>
       </c>
@@ -2066,14 +2048,14 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="L39" s="25"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F40" s="25"/>
       <c r="L40" s="25"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="28" t="s">
         <v>121</v>
       </c>
@@ -2081,9 +2063,6 @@
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
       <c r="F42" s="30"/>
-      <c r="G42" t="s">
-        <v>145</v>
-      </c>
       <c r="H42" s="28" t="s">
         <v>120</v>
       </c>
@@ -2091,11 +2070,8 @@
       <c r="J42" s="29"/>
       <c r="K42" s="29"/>
       <c r="L42" s="30"/>
-      <c r="M42" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>0</v>
       </c>
@@ -2125,7 +2101,7 @@
       </c>
       <c r="L43" s="23"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>17</v>
       </c>
@@ -2151,7 +2127,7 @@
       </c>
       <c r="L44" s="24"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>37</v>
       </c>
@@ -2177,7 +2153,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="23"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H46" s="1" t="s">
         <v>34</v>
       </c>
@@ -2190,7 +2166,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="23"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H47" s="1" t="s">
         <v>35</v>
       </c>
@@ -2203,7 +2179,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="23"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H48" s="19" t="s">
         <v>36</v>
       </c>
@@ -2220,20 +2196,17 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F50" s="25"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
       <c r="E52" s="29"/>
       <c r="F52" s="30"/>
-      <c r="G52" t="s">
-        <v>145</v>
-      </c>
       <c r="H52" s="31" t="s">
         <v>116</v>
       </c>
@@ -2241,11 +2214,8 @@
       <c r="J52" s="31"/>
       <c r="K52" s="31"/>
       <c r="L52" s="31"/>
-      <c r="M52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>0</v>
       </c>
@@ -2273,7 +2243,7 @@
       </c>
       <c r="L53" s="23"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>21</v>
       </c>
@@ -2299,7 +2269,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="23"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
         <v>31</v>
       </c>
@@ -2325,7 +2295,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
renaming services to subscriptions, providedServices to offers
</commit_message>
<xml_diff>
--- a/doc/prj.xlsx
+++ b/doc/prj.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\Java\Station\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="19320" windowHeight="7995"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="150">
   <si>
     <t>id</t>
   </si>
@@ -435,7 +440,48 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">services </t>
+      <t xml:space="preserve">subscribers </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* абоненты */</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">calls </t>
     </r>
     <r>
       <rPr>
@@ -471,12 +517,12 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/* подключенные услуги */</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">subscribers </t>
+      <t>/* звонки */</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">calling_rates </t>
     </r>
     <r>
       <rPr>
@@ -512,12 +558,45 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/* абоненты */</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">provided_services  </t>
+      <t>/* тарифы на звонки */</t>
+    </r>
+  </si>
+  <si>
+    <t>isActive</t>
+  </si>
+  <si>
+    <t>surname</t>
+  </si>
+  <si>
+    <t>patronymic</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>prefixID</t>
+  </si>
+  <si>
+    <t>passportID</t>
+  </si>
+  <si>
+    <t>personalID</t>
+  </si>
+  <si>
+    <t>личный номер сотрудника</t>
+  </si>
+  <si>
+    <t>true|false активен|заблокирован</t>
+  </si>
+  <si>
+    <t>префикс тел. номера</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">prefixes </t>
     </r>
     <r>
       <rPr>
@@ -553,12 +632,145 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/* предоставляемые услуги */</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">calls </t>
+      <t>/* префиксы телефонных номеров</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*/</t>
+    </r>
+  </si>
+  <si>
+    <t>город</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">administrators </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/*список администраторов */</t>
+    </r>
+  </si>
+  <si>
+    <t>идентификационный номер паспорта</t>
+  </si>
+  <si>
+    <t>NN, UQ(сост)</t>
+  </si>
+  <si>
+    <t>префикс тел. номера, составной уникальный ключ</t>
+  </si>
+  <si>
+    <t>телефонный номер, составной уникальный ключ</t>
+  </si>
+  <si>
+    <t>0101ASJL2</t>
+  </si>
+  <si>
+    <t>0101ASJL3</t>
+  </si>
+  <si>
+    <t>surname+name+patronymic</t>
+  </si>
+  <si>
+    <t>210045, ул. Полярная, д. 1</t>
+  </si>
+  <si>
+    <t>210007, ул. Заполярная, д. 2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">invoices </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CRUD </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* счета */</t>
+    </r>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>java type: float; абонентская плата в мес</t>
+  </si>
+  <si>
+    <t>java type: float; стоимость подключения</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">subscriptions </t>
     </r>
     <r>
       <rPr>
@@ -594,12 +806,12 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/* звонки */</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">calling_rates </t>
+      <t>/* подключенные услуги */</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">offers  </t>
     </r>
     <r>
       <rPr>
@@ -635,221 +847,17 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/* тарифы на звонки */</t>
-    </r>
-  </si>
-  <si>
-    <t>isActive</t>
-  </si>
-  <si>
-    <t>surname</t>
-  </si>
-  <si>
-    <t>patronymic</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>prefixID</t>
-  </si>
-  <si>
-    <t>passportID</t>
-  </si>
-  <si>
-    <t>personalID</t>
-  </si>
-  <si>
-    <t>личный номер сотрудника</t>
-  </si>
-  <si>
-    <t>true|false активен|заблокирован</t>
-  </si>
-  <si>
-    <t>префикс тел. номера</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">prefixes </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRUD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/* префиксы телефонных номеров</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*/</t>
-    </r>
-  </si>
-  <si>
-    <t>город</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">administrators </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CRUD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/*список администраторов */</t>
-    </r>
-  </si>
-  <si>
-    <t>идентификационный номер паспорта</t>
-  </si>
-  <si>
-    <t>NN, UQ(сост)</t>
-  </si>
-  <si>
-    <t>префикс тел. номера, составной уникальный ключ</t>
-  </si>
-  <si>
-    <t>телефонный номер, составной уникальный ключ</t>
-  </si>
-  <si>
-    <t>0101ASJL2</t>
-  </si>
-  <si>
-    <t>0101ASJL3</t>
-  </si>
-  <si>
-    <t>surname+name+patronymic</t>
-  </si>
-  <si>
-    <t>210045, ул. Полярная, д. 1</t>
-  </si>
-  <si>
-    <t>210007, ул. Заполярная, д. 2</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">invoices </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">CRUD </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/* счета */</t>
-    </r>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>java type: float; абонентская плата в мес</t>
-  </si>
-  <si>
-    <t>java type: float; стоимость подключения</t>
+      <t>/* предоставляемые услуги */</t>
+    </r>
+  </si>
+  <si>
+    <t>offerID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1229,7 +1237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1262,9 +1270,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1297,6 +1322,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1475,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1578,7 @@
       <c r="E4" s="29"/>
       <c r="F4" s="30"/>
       <c r="G4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -1586,7 +1628,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>103</v>
@@ -1612,7 +1654,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>103</v>
@@ -1640,7 +1682,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>112</v>
@@ -1650,32 +1692,32 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" s="36"/>
       <c r="D16" s="36"/>
       <c r="E16" s="36"/>
       <c r="F16" s="37"/>
       <c r="G16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I16" s="33"/>
       <c r="J16" s="33"/>
       <c r="K16" s="33"/>
       <c r="L16" s="34"/>
       <c r="M16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>0</v>
       </c>
@@ -1703,9 +1745,9 @@
       </c>
       <c r="L17" s="24"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>92</v>
@@ -1715,10 +1757,10 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>102</v>
@@ -1728,10 +1770,10 @@
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1757,7 +1799,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="27"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H20" s="1" t="s">
         <v>15</v>
       </c>
@@ -1770,24 +1812,24 @@
       <c r="K20" s="1"/>
       <c r="L20" s="27"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H21" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>92</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K21" s="19" t="s">
         <v>13</v>
       </c>
       <c r="L21" s="24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H22" s="1" t="s">
         <v>38</v>
       </c>
@@ -1795,14 +1837,14 @@
         <v>92</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="27" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H23" s="19" t="s">
         <v>86</v>
       </c>
@@ -1819,18 +1861,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C26" s="36"/>
       <c r="D26" s="36"/>
       <c r="E26" s="36"/>
       <c r="F26" s="37"/>
     </row>
-    <row r="27" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>92</v>
@@ -1842,12 +1884,12 @@
         <v>12</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>102</v>
@@ -1857,27 +1899,30 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="37"/>
       <c r="G32" t="s">
-        <v>146</v>
-      </c>
-      <c r="H32" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="30"/>
+        <v>144</v>
+      </c>
+      <c r="H32" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="37"/>
+      <c r="M32" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
@@ -1945,8 +1990,8 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="23"/>
-      <c r="H35" s="19" t="s">
-        <v>22</v>
+      <c r="H35" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="I35" s="19" t="s">
         <v>92</v>
@@ -1971,7 +2016,7 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>24</v>
@@ -1999,7 +2044,7 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>25</v>
@@ -2039,14 +2084,14 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C42" s="29"/>
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
       <c r="F42" s="30"/>
       <c r="H42" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I42" s="29"/>
       <c r="J42" s="29"/>
@@ -2183,7 +2228,7 @@
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
@@ -2371,13 +2416,13 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2456,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>10</v>
@@ -2465,7 +2510,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>38</v>
@@ -2479,13 +2524,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D11" s="6">
         <v>29566</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F11" s="1">
         <v>212</v>
@@ -2502,13 +2547,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D12" s="6">
         <v>28105</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F12" s="1">
         <v>17</v>
@@ -2532,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
bugfix replace invoice.`amout` to decimal(10,4)
</commit_message>
<xml_diff>
--- a/doc/prj.xlsx
+++ b/doc/prj.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\Java\Station\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="19320" windowHeight="7995"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="102">
   <si>
     <t>id</t>
   </si>
@@ -687,12 +682,18 @@
   </si>
   <si>
     <t>дата и время завершения звонка</t>
+  </si>
+  <si>
+    <t>DECIMAL(10,4)</t>
+  </si>
+  <si>
+    <t>java type: bigDecimal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -888,6 +889,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -917,12 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -985,7 +986,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1018,26 +1019,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1070,23 +1054,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1265,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,13 +1285,13 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
       <c r="G4" t="s">
         <v>84</v>
       </c>
@@ -1444,23 +1411,23 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
       <c r="G16" t="s">
         <v>84</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="26"/>
       <c r="M16" t="s">
         <v>84</v>
       </c>
@@ -1610,13 +1577,13 @@
       </c>
     </row>
     <row r="26" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
     </row>
     <row r="27" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
@@ -1651,23 +1618,23 @@
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22"/>
       <c r="G32" t="s">
         <v>84</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="20"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="22"/>
       <c r="M32" t="s">
         <v>84</v>
       </c>
@@ -1831,23 +1798,23 @@
       <c r="L40" s="12"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="17"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="19"/>
       <c r="G42" t="s">
         <v>84</v>
       </c>
-      <c r="H42" s="15" t="s">
+      <c r="H42" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="17"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="19"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -1880,17 +1847,17 @@
       <c r="L43" s="10"/>
     </row>
     <row r="44" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D44" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="26" t="s">
+      <c r="D44" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="F44" s="16" t="s">
         <v>96</v>
       </c>
       <c r="H44" s="6" t="s">
@@ -2010,20 +1977,20 @@
       <c r="L49" s="11"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="17"/>
-      <c r="H53" s="21" t="s">
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="19"/>
+      <c r="H53" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
-      <c r="K53" s="21"/>
-      <c r="L53" s="21"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
+      <c r="K53" s="23"/>
+      <c r="L53" s="23"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
@@ -2109,15 +2076,15 @@
       <c r="B57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>48</v>
+      <c r="C57" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="10" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>36</v>

</xml_diff>